<commit_message>
updated risk register template
</commit_message>
<xml_diff>
--- a/templates/2.4.1_RiskRegisterTemplate.xlsx
+++ b/templates/2.4.1_RiskRegisterTemplate.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/496d41b51a3bd866/PMI Case Challenge/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding Projects\PMI_CaseStudyChallenge\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{337E05BD-3BEF-444B-9001-4A78062B75EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F50D02C8-B42C-444F-ACD6-D728DE31968D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF96F92-20E3-4AAB-8DF2-36B8FC5E5233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{10DC767F-9AC1-4A15-B30C-1E1DA7DCE18C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10DC767F-9AC1-4A15-B30C-1E1DA7DCE18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Risk Register" sheetId="1" r:id="rId1"/>
-    <sheet name="Priority Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -208,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -579,19 +578,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -619,17 +605,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -713,47 +688,156 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -763,157 +847,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,149 +1214,117 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="24" style="13" customWidth="1"/>
-    <col min="6" max="6" width="22" style="13" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="24" style="12" customWidth="1"/>
+    <col min="6" max="6" width="22" style="12" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="12" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3"/>
+      <c r="H3"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
+      <c r="G4"/>
+      <c r="H4"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5"/>
+      <c r="H5"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6"/>
+      <c r="H6"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7"/>
+      <c r="H7"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+      <c r="G8"/>
+      <c r="H8"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="G9"/>
+      <c r="H9"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10"/>
+      <c r="H10"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11"/>
@@ -1418,291 +1336,291 @@
       <c r="H11"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="53"/>
     </row>
     <row r="13" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="40">
+      <c r="K14" s="29">
         <v>5</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="19">
         <v>5</v>
       </c>
-      <c r="M14" s="34">
+      <c r="M14" s="23">
         <v>10</v>
       </c>
-      <c r="N14" s="39">
+      <c r="N14" s="28">
         <v>15</v>
       </c>
-      <c r="O14" s="39">
+      <c r="O14" s="28">
         <v>20</v>
       </c>
-      <c r="P14" s="33">
+      <c r="P14" s="22">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="41">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="30">
         <v>4</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="20">
         <v>4</v>
       </c>
-      <c r="M15" s="35">
+      <c r="M15" s="24">
         <v>8</v>
       </c>
-      <c r="N15" s="35">
+      <c r="N15" s="24">
         <v>12</v>
       </c>
-      <c r="O15" s="38">
+      <c r="O15" s="27">
         <v>16</v>
       </c>
-      <c r="P15" s="37">
+      <c r="P15" s="26">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="41">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="30">
         <v>3</v>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="20">
         <v>3</v>
       </c>
-      <c r="M16" s="35">
+      <c r="M16" s="24">
         <v>6</v>
       </c>
-      <c r="N16" s="35">
+      <c r="N16" s="24">
         <v>9</v>
       </c>
-      <c r="O16" s="35">
+      <c r="O16" s="24">
         <v>12</v>
       </c>
-      <c r="P16" s="37">
+      <c r="P16" s="26">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="41">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="30">
         <v>2</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="20">
         <v>2</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M17" s="20">
         <v>4</v>
       </c>
-      <c r="N17" s="35">
+      <c r="N17" s="24">
         <v>6</v>
       </c>
-      <c r="O17" s="35">
+      <c r="O17" s="24">
         <v>8</v>
       </c>
-      <c r="P17" s="36">
+      <c r="P17" s="25">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="41">
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="30">
         <v>1</v>
       </c>
-      <c r="L18" s="31">
+      <c r="L18" s="20">
         <v>1</v>
       </c>
-      <c r="M18" s="31">
+      <c r="M18" s="20">
         <v>2</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="20">
         <v>3</v>
       </c>
-      <c r="O18" s="31">
+      <c r="O18" s="20">
         <v>4</v>
       </c>
-      <c r="P18" s="32">
+      <c r="P18" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="42">
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="31">
         <v>1</v>
       </c>
-      <c r="M19" s="42">
+      <c r="M19" s="31">
         <v>2</v>
       </c>
-      <c r="N19" s="42">
+      <c r="N19" s="31">
         <v>3</v>
       </c>
-      <c r="O19" s="42">
+      <c r="O19" s="31">
         <v>4</v>
       </c>
-      <c r="P19" s="43">
+      <c r="P19" s="32">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-      <c r="K20" s="44" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="K20" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="46"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="56"/>
     </row>
     <row r="21" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
     </row>
     <row r="27" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1712,169 +1630,16 @@
     <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="K20:P20"/>
+    <mergeCell ref="J14:J19"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="K20:P20"/>
-    <mergeCell ref="J14:J19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC17916-B471-45CB-8212-D6A302E39A6A}">
-  <dimension ref="B4:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="8" width="8.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="23">
-        <v>5</v>
-      </c>
-      <c r="D5" s="23">
-        <v>5</v>
-      </c>
-      <c r="E5" s="23">
-        <v>10</v>
-      </c>
-      <c r="F5" s="24">
-        <v>15</v>
-      </c>
-      <c r="G5" s="25">
-        <v>20</v>
-      </c>
-      <c r="H5" s="25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="26">
-        <v>4</v>
-      </c>
-      <c r="D6" s="26">
-        <v>4</v>
-      </c>
-      <c r="E6" s="26">
-        <v>8</v>
-      </c>
-      <c r="F6" s="27">
-        <v>12</v>
-      </c>
-      <c r="G6" s="28">
-        <v>16</v>
-      </c>
-      <c r="H6" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="26">
-        <v>3</v>
-      </c>
-      <c r="D7" s="26">
-        <v>3</v>
-      </c>
-      <c r="E7" s="26">
-        <v>6</v>
-      </c>
-      <c r="F7" s="27">
-        <v>9</v>
-      </c>
-      <c r="G7" s="28">
-        <v>12</v>
-      </c>
-      <c r="H7" s="28">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="26">
-        <v>2</v>
-      </c>
-      <c r="D8" s="26">
-        <v>2</v>
-      </c>
-      <c r="E8" s="26">
-        <v>4</v>
-      </c>
-      <c r="F8" s="27">
-        <v>6</v>
-      </c>
-      <c r="G8" s="28">
-        <v>8</v>
-      </c>
-      <c r="H8" s="28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="26">
-        <v>1</v>
-      </c>
-      <c r="D9" s="27">
-        <v>1</v>
-      </c>
-      <c r="E9" s="29">
-        <v>2</v>
-      </c>
-      <c r="F9" s="27">
-        <v>3</v>
-      </c>
-      <c r="G9" s="28">
-        <v>4</v>
-      </c>
-      <c r="H9" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="27"/>
-      <c r="D10" s="27">
-        <v>1</v>
-      </c>
-      <c r="E10" s="27">
-        <v>2</v>
-      </c>
-      <c r="F10" s="27">
-        <v>3</v>
-      </c>
-      <c r="G10" s="27">
-        <v>4</v>
-      </c>
-      <c r="H10" s="27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="B5:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>